<commit_message>
Adding codes for HMW analysis, not yet activated
</commit_message>
<xml_diff>
--- a/inst/extdata/FAO_ISO_MW_Mapping.xlsx
+++ b/inst/extdata/FAO_ISO_MW_Mapping.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="461">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -1375,6 +1375,30 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>HMW.Region.code</t>
+  </si>
+  <si>
+    <t>MENA</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>SSA</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>WO</t>
+  </si>
+  <si>
+    <t>WE</t>
+  </si>
+  <si>
+    <t>SSEA</t>
   </si>
   <si>
     <t>MW.Region.code</t>
@@ -2183,10 +2207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E240"/>
+  <dimension ref="A1:F240"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2195,10 +2219,11 @@
     <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>448</v>
       </c>
@@ -2212,10 +2237,13 @@
         <v>278</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2228,8 +2256,11 @@
       <c r="E2" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2242,8 +2273,11 @@
       <c r="E3" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2256,8 +2290,11 @@
       <c r="E4" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2270,8 +2307,11 @@
       <c r="E5" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2284,8 +2324,11 @@
       <c r="E6" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2298,8 +2341,11 @@
       <c r="E7" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2312,8 +2358,11 @@
       <c r="E8" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2326,8 +2375,11 @@
       <c r="E9" s="1" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2340,8 +2392,11 @@
       <c r="E10" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2354,8 +2409,11 @@
       <c r="E11" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2368,8 +2426,11 @@
       <c r="E12" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2382,8 +2443,11 @@
       <c r="E13" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2396,8 +2460,11 @@
       <c r="E14" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2410,8 +2477,11 @@
       <c r="E15" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2424,8 +2494,11 @@
       <c r="E16" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -2438,8 +2511,11 @@
       <c r="E17" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -2452,8 +2528,11 @@
       <c r="E18" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -2466,8 +2545,11 @@
       <c r="E19" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -2480,8 +2562,11 @@
       <c r="E20" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -2494,8 +2579,11 @@
       <c r="E21" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -2508,8 +2596,11 @@
       <c r="E22" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -2522,8 +2613,11 @@
       <c r="E23" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -2536,8 +2630,11 @@
       <c r="E24" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -2550,8 +2647,11 @@
       <c r="E25" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -2564,8 +2664,11 @@
       <c r="E26" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -2578,8 +2681,11 @@
       <c r="E27" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -2592,8 +2698,11 @@
       <c r="E28" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -2606,8 +2715,11 @@
       <c r="E29" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -2620,8 +2732,11 @@
       <c r="E30" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -2634,8 +2749,11 @@
       <c r="E31" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -2648,8 +2766,11 @@
       <c r="E32" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -2662,8 +2783,11 @@
       <c r="E33" s="1" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -2676,8 +2800,11 @@
       <c r="E34" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -2690,8 +2817,11 @@
       <c r="E35" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -2704,8 +2834,11 @@
       <c r="E36" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -2718,8 +2851,11 @@
       <c r="E37" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -2732,8 +2868,11 @@
       <c r="E38" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -2746,8 +2885,11 @@
       <c r="E39" s="1" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -2760,8 +2902,11 @@
       <c r="E40" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -2774,8 +2919,11 @@
       <c r="E41" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -2788,8 +2936,11 @@
       <c r="E42" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -2802,8 +2953,11 @@
       <c r="E43" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -2816,8 +2970,11 @@
       <c r="E44" s="1" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -2830,8 +2987,11 @@
       <c r="E45" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -2844,8 +3004,11 @@
       <c r="E46" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
@@ -2858,8 +3021,11 @@
       <c r="E47" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -2872,8 +3038,11 @@
       <c r="E48" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -2886,8 +3055,11 @@
       <c r="E49" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -2900,8 +3072,11 @@
       <c r="E50" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -2914,8 +3089,11 @@
       <c r="E51" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
@@ -2928,8 +3106,11 @@
       <c r="E52" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
@@ -2942,8 +3123,11 @@
       <c r="E53" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
@@ -2956,8 +3140,11 @@
       <c r="E54" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
@@ -2970,8 +3157,11 @@
       <c r="E55" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
@@ -2984,8 +3174,11 @@
       <c r="E56" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
@@ -2998,8 +3191,11 @@
       <c r="E57" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
@@ -3012,8 +3208,11 @@
       <c r="E58" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
@@ -3026,8 +3225,11 @@
       <c r="E59" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
@@ -3040,8 +3242,11 @@
       <c r="E60" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
@@ -3054,8 +3259,11 @@
       <c r="E61" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
@@ -3068,8 +3276,11 @@
       <c r="E62" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
@@ -3082,8 +3293,11 @@
       <c r="E63" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
@@ -3096,8 +3310,11 @@
       <c r="E64" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>63</v>
       </c>
@@ -3110,8 +3327,11 @@
       <c r="E65" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>64</v>
       </c>
@@ -3124,8 +3344,11 @@
       <c r="E66" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
@@ -3138,8 +3361,11 @@
       <c r="E67" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
@@ -3152,8 +3378,11 @@
       <c r="E68" s="1" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
@@ -3166,8 +3395,11 @@
       <c r="E69" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
@@ -3180,8 +3412,11 @@
       <c r="E70" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
@@ -3194,8 +3429,11 @@
       <c r="E71" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
@@ -3208,8 +3446,11 @@
       <c r="E72" s="1" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
@@ -3222,8 +3463,11 @@
       <c r="E73" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
@@ -3236,8 +3480,11 @@
       <c r="E74" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
@@ -3250,8 +3497,11 @@
       <c r="E75" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
@@ -3264,8 +3514,11 @@
       <c r="E76" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
@@ -3278,8 +3531,11 @@
       <c r="E77" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
@@ -3292,8 +3548,11 @@
       <c r="E78" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
@@ -3306,8 +3565,11 @@
       <c r="E79" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
@@ -3320,8 +3582,11 @@
       <c r="E80" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>79</v>
       </c>
@@ -3334,8 +3599,11 @@
       <c r="E81" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>80</v>
       </c>
@@ -3348,8 +3616,11 @@
       <c r="E82" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>81</v>
       </c>
@@ -3362,8 +3633,11 @@
       <c r="E83" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
@@ -3376,8 +3650,11 @@
       <c r="E84" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>83</v>
       </c>
@@ -3390,8 +3667,11 @@
       <c r="E85" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>84</v>
       </c>
@@ -3404,8 +3684,11 @@
       <c r="E86" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
@@ -3418,8 +3701,11 @@
       <c r="E87" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
@@ -3432,8 +3718,11 @@
       <c r="E88" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>87</v>
       </c>
@@ -3446,8 +3735,11 @@
       <c r="E89" s="1" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>88</v>
       </c>
@@ -3460,8 +3752,11 @@
       <c r="E90" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>89</v>
       </c>
@@ -3474,8 +3769,11 @@
       <c r="E91" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
@@ -3488,8 +3786,11 @@
       <c r="E92" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
@@ -3502,8 +3803,11 @@
       <c r="E93" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
@@ -3516,8 +3820,11 @@
       <c r="E94" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>93</v>
       </c>
@@ -3530,8 +3837,11 @@
       <c r="E95" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
@@ -3544,8 +3854,11 @@
       <c r="E96" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>95</v>
       </c>
@@ -3558,8 +3871,11 @@
       <c r="E97" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>96</v>
       </c>
@@ -3572,8 +3888,11 @@
       <c r="E98" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>97</v>
       </c>
@@ -3586,8 +3905,11 @@
       <c r="E99" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
@@ -3600,8 +3922,11 @@
       <c r="E100" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>99</v>
       </c>
@@ -3614,8 +3939,11 @@
       <c r="E101" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>100</v>
       </c>
@@ -3628,8 +3956,11 @@
       <c r="E102" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>101</v>
       </c>
@@ -3642,8 +3973,11 @@
       <c r="E103" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F103" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>102</v>
       </c>
@@ -3656,8 +3990,11 @@
       <c r="E104" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F104" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>103</v>
       </c>
@@ -3670,8 +4007,11 @@
       <c r="E105" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F105" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>104</v>
       </c>
@@ -3684,8 +4024,11 @@
       <c r="E106" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F106" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>105</v>
       </c>
@@ -3698,8 +4041,11 @@
       <c r="E107" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F107" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>106</v>
       </c>
@@ -3712,8 +4058,11 @@
       <c r="E108" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F108" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>107</v>
       </c>
@@ -3726,8 +4075,11 @@
       <c r="E109" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F109" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>108</v>
       </c>
@@ -3740,8 +4092,11 @@
       <c r="E110" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F110" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>109</v>
       </c>
@@ -3754,8 +4109,11 @@
       <c r="E111" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F111" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>110</v>
       </c>
@@ -3768,8 +4126,11 @@
       <c r="E112" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F112" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>111</v>
       </c>
@@ -3782,8 +4143,11 @@
       <c r="E113" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F113" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>112</v>
       </c>
@@ -3796,8 +4160,11 @@
       <c r="E114" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F114" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>113</v>
       </c>
@@ -3810,8 +4177,11 @@
       <c r="E115" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F115" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>114</v>
       </c>
@@ -3824,8 +4194,11 @@
       <c r="E116" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F116" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>115</v>
       </c>
@@ -3838,8 +4211,11 @@
       <c r="E117" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F117" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>116</v>
       </c>
@@ -3852,8 +4228,11 @@
       <c r="E118" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F118" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>117</v>
       </c>
@@ -3866,8 +4245,11 @@
       <c r="E119" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F119" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>118</v>
       </c>
@@ -3880,8 +4262,11 @@
       <c r="E120" s="1" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F120" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>119</v>
       </c>
@@ -3894,8 +4279,11 @@
       <c r="E121" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F121" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>120</v>
       </c>
@@ -3908,8 +4296,11 @@
       <c r="E122" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F122" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>121</v>
       </c>
@@ -3922,8 +4313,11 @@
       <c r="E123" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F123" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>122</v>
       </c>
@@ -3936,8 +4330,11 @@
       <c r="E124" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F124" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>123</v>
       </c>
@@ -3950,8 +4347,11 @@
       <c r="E125" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F125" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>124</v>
       </c>
@@ -3964,8 +4364,11 @@
       <c r="E126" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F126" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>125</v>
       </c>
@@ -3978,8 +4381,11 @@
       <c r="E127" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F127" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>126</v>
       </c>
@@ -3992,8 +4398,11 @@
       <c r="E128" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F128" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>127</v>
       </c>
@@ -4006,8 +4415,11 @@
       <c r="E129" s="1" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F129" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>128</v>
       </c>
@@ -4020,8 +4432,11 @@
       <c r="E130" s="1" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F130" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>129</v>
       </c>
@@ -4034,8 +4449,11 @@
       <c r="E131" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F131" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>130</v>
       </c>
@@ -4048,8 +4466,11 @@
       <c r="E132" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F132" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>131</v>
       </c>
@@ -4062,8 +4483,11 @@
       <c r="E133" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F133" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>132</v>
       </c>
@@ -4076,8 +4500,11 @@
       <c r="E134" s="1" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F134" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>133</v>
       </c>
@@ -4090,8 +4517,11 @@
       <c r="E135" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F135" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>134</v>
       </c>
@@ -4104,8 +4534,11 @@
       <c r="E136" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F136" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>135</v>
       </c>
@@ -4118,8 +4551,11 @@
       <c r="E137" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F137" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>136</v>
       </c>
@@ -4132,8 +4568,11 @@
       <c r="E138" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F138" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>137</v>
       </c>
@@ -4146,8 +4585,11 @@
       <c r="E139" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F139" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>138</v>
       </c>
@@ -4160,8 +4602,11 @@
       <c r="E140" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F140" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>139</v>
       </c>
@@ -4174,8 +4619,11 @@
       <c r="E141" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F141" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>140</v>
       </c>
@@ -4188,8 +4636,11 @@
       <c r="E142" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F142" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>141</v>
       </c>
@@ -4202,8 +4653,11 @@
       <c r="E143" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F143" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>142</v>
       </c>
@@ -4216,8 +4670,11 @@
       <c r="E144" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F144" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>143</v>
       </c>
@@ -4230,8 +4687,11 @@
       <c r="E145" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F145" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>144</v>
       </c>
@@ -4244,8 +4704,11 @@
       <c r="E146" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F146" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>145</v>
       </c>
@@ -4258,8 +4721,11 @@
       <c r="E147" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F147" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>146</v>
       </c>
@@ -4272,8 +4738,11 @@
       <c r="E148" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F148" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>147</v>
       </c>
@@ -4286,8 +4755,11 @@
       <c r="E149" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F149" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>148</v>
       </c>
@@ -4300,8 +4772,11 @@
       <c r="E150" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F150" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>149</v>
       </c>
@@ -4314,8 +4789,11 @@
       <c r="E151" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F151" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>150</v>
       </c>
@@ -4328,8 +4806,11 @@
       <c r="E152" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F152" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>151</v>
       </c>
@@ -4342,8 +4823,11 @@
       <c r="E153" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F153" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>152</v>
       </c>
@@ -4356,8 +4840,11 @@
       <c r="E154" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F154" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>153</v>
       </c>
@@ -4370,8 +4857,11 @@
       <c r="E155" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F155" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>154</v>
       </c>
@@ -4384,8 +4874,11 @@
       <c r="E156" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F156" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>155</v>
       </c>
@@ -4398,8 +4891,11 @@
       <c r="E157" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F157" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>156</v>
       </c>
@@ -4412,8 +4908,11 @@
       <c r="E158" s="1" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F158" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>157</v>
       </c>
@@ -4426,8 +4925,11 @@
       <c r="E159" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F159" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>158</v>
       </c>
@@ -4440,8 +4942,11 @@
       <c r="E160" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F160" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>159</v>
       </c>
@@ -4454,8 +4959,11 @@
       <c r="E161" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F161" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>160</v>
       </c>
@@ -4468,8 +4976,11 @@
       <c r="E162" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F162" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>161</v>
       </c>
@@ -4482,8 +4993,11 @@
       <c r="E163" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F163" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>162</v>
       </c>
@@ -4496,8 +5010,11 @@
       <c r="E164" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F164" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>163</v>
       </c>
@@ -4510,8 +5027,11 @@
       <c r="E165" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F165" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>164</v>
       </c>
@@ -4524,8 +5044,11 @@
       <c r="E166" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F166" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>165</v>
       </c>
@@ -4538,8 +5061,11 @@
       <c r="E167" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F167" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>166</v>
       </c>
@@ -4552,8 +5078,11 @@
       <c r="E168" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F168" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>167</v>
       </c>
@@ -4566,8 +5095,11 @@
       <c r="E169" s="1" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F169" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>168</v>
       </c>
@@ -4580,8 +5112,11 @@
       <c r="E170" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F170" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>169</v>
       </c>
@@ -4594,8 +5129,11 @@
       <c r="E171" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F171" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>170</v>
       </c>
@@ -4608,8 +5146,11 @@
       <c r="E172" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F172" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>171</v>
       </c>
@@ -4622,8 +5163,11 @@
       <c r="E173" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F173" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>172</v>
       </c>
@@ -4636,8 +5180,11 @@
       <c r="E174" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F174" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>173</v>
       </c>
@@ -4650,8 +5197,11 @@
       <c r="E175" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F175" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>174</v>
       </c>
@@ -4664,8 +5214,11 @@
       <c r="E176" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F176" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>175</v>
       </c>
@@ -4678,8 +5231,11 @@
       <c r="E177" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F177" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>176</v>
       </c>
@@ -4692,8 +5248,11 @@
       <c r="E178" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F178" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>177</v>
       </c>
@@ -4706,8 +5265,11 @@
       <c r="E179" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F179" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>178</v>
       </c>
@@ -4720,8 +5282,11 @@
       <c r="E180" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F180" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>179</v>
       </c>
@@ -4734,8 +5299,11 @@
       <c r="E181" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F181" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>180</v>
       </c>
@@ -4748,8 +5316,11 @@
       <c r="E182" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F182" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>181</v>
       </c>
@@ -4762,8 +5333,11 @@
       <c r="E183" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F183" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>182</v>
       </c>
@@ -4776,8 +5350,11 @@
       <c r="E184" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F184" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>183</v>
       </c>
@@ -4790,8 +5367,11 @@
       <c r="E185" s="1" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F185" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>184</v>
       </c>
@@ -4804,8 +5384,11 @@
       <c r="E186" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F186" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>185</v>
       </c>
@@ -4818,8 +5401,11 @@
       <c r="E187" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F187" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>186</v>
       </c>
@@ -4832,8 +5418,11 @@
       <c r="E188" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F188" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>187</v>
       </c>
@@ -4846,8 +5435,11 @@
       <c r="E189" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F189" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>188</v>
       </c>
@@ -4860,8 +5452,11 @@
       <c r="E190" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F190" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>189</v>
       </c>
@@ -4874,8 +5469,11 @@
       <c r="E191" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F191" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>190</v>
       </c>
@@ -4888,8 +5486,11 @@
       <c r="E192" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F192" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>191</v>
       </c>
@@ -4902,8 +5503,11 @@
       <c r="E193" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F193" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>192</v>
       </c>
@@ -4916,8 +5520,11 @@
       <c r="E194" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F194" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>193</v>
       </c>
@@ -4930,8 +5537,11 @@
       <c r="E195" s="1" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F195" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>194</v>
       </c>
@@ -4944,8 +5554,11 @@
       <c r="E196" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F196" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>195</v>
       </c>
@@ -4958,8 +5571,11 @@
       <c r="E197" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F197" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>196</v>
       </c>
@@ -4972,8 +5588,11 @@
       <c r="E198" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F198" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>197</v>
       </c>
@@ -4986,8 +5605,11 @@
       <c r="E199" s="1" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F199" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>198</v>
       </c>
@@ -5000,8 +5622,11 @@
       <c r="E200" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F200" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>199</v>
       </c>
@@ -5014,8 +5639,11 @@
       <c r="E201" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F201" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>200</v>
       </c>
@@ -5028,8 +5656,11 @@
       <c r="E202" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F202" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>201</v>
       </c>
@@ -5042,8 +5673,11 @@
       <c r="E203" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F203" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>202</v>
       </c>
@@ -5056,8 +5690,11 @@
       <c r="E204" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F204" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>203</v>
       </c>
@@ -5070,8 +5707,11 @@
       <c r="E205" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F205" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>204</v>
       </c>
@@ -5085,7 +5725,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>205</v>
       </c>
@@ -5099,7 +5739,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>206</v>
       </c>

</xml_diff>

<commit_message>
bundling fao data, tests working, separated amw and hmw region code cols
</commit_message>
<xml_diff>
--- a/inst/extdata/FAO_ISO_MW_Mapping.xlsx
+++ b/inst/extdata/FAO_ISO_MW_Mapping.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="461">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -1401,7 +1401,7 @@
     <t>SSEA</t>
   </si>
   <si>
-    <t>MW.Region.code</t>
+    <t>AMW.Region.code</t>
   </si>
 </sst>
 </file>
@@ -2210,7 +2210,7 @@
   <dimension ref="A1:F240"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F206" sqref="F206:F240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5724,6 +5724,9 @@
       <c r="E206" s="1" t="s">
         <v>282</v>
       </c>
+      <c r="F206" s="1" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
@@ -5738,6 +5741,9 @@
       <c r="E207" s="1" t="s">
         <v>282</v>
       </c>
+      <c r="F207" s="1" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
@@ -5752,8 +5758,11 @@
       <c r="E208" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F208" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>207</v>
       </c>
@@ -5766,8 +5775,11 @@
       <c r="E209" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F209" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>208</v>
       </c>
@@ -5780,8 +5792,11 @@
       <c r="E210" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F210" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>209</v>
       </c>
@@ -5794,8 +5809,11 @@
       <c r="E211" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F211" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>210</v>
       </c>
@@ -5808,8 +5826,11 @@
       <c r="E212" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F212" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>211</v>
       </c>
@@ -5822,8 +5843,11 @@
       <c r="E213" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F213" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>212</v>
       </c>
@@ -5836,8 +5860,11 @@
       <c r="E214" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F214" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>213</v>
       </c>
@@ -5850,8 +5877,11 @@
       <c r="E215" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F215" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>214</v>
       </c>
@@ -5864,8 +5894,11 @@
       <c r="E216" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F216" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>215</v>
       </c>
@@ -5878,8 +5911,11 @@
       <c r="E217" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F217" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>216</v>
       </c>
@@ -5892,8 +5928,11 @@
       <c r="E218" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F218" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>217</v>
       </c>
@@ -5906,8 +5945,11 @@
       <c r="E219" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F219" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>218</v>
       </c>
@@ -5920,8 +5962,11 @@
       <c r="E220" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F220" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>219</v>
       </c>
@@ -5934,8 +5979,11 @@
       <c r="E221" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F221" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>220</v>
       </c>
@@ -5948,8 +5996,11 @@
       <c r="E222" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F222" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>221</v>
       </c>
@@ -5962,8 +6013,11 @@
       <c r="E223" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F223" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>222</v>
       </c>
@@ -5976,8 +6030,11 @@
       <c r="E224" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F224" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>223</v>
       </c>
@@ -5990,8 +6047,11 @@
       <c r="E225" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F225" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>224</v>
       </c>
@@ -6004,8 +6064,11 @@
       <c r="E226" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F226" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>225</v>
       </c>
@@ -6018,8 +6081,11 @@
       <c r="E227" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F227" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>226</v>
       </c>
@@ -6032,8 +6098,11 @@
       <c r="E228" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F228" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>227</v>
       </c>
@@ -6046,8 +6115,11 @@
       <c r="E229" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F229" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>228</v>
       </c>
@@ -6060,8 +6132,11 @@
       <c r="E230" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F230" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>229</v>
       </c>
@@ -6074,8 +6149,11 @@
       <c r="E231" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F231" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>230</v>
       </c>
@@ -6088,8 +6166,11 @@
       <c r="E232" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F232" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>231</v>
       </c>
@@ -6102,8 +6183,11 @@
       <c r="E233" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F233" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>232</v>
       </c>
@@ -6116,8 +6200,11 @@
       <c r="E234" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F234" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>233</v>
       </c>
@@ -6130,8 +6217,11 @@
       <c r="E235" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F235" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>234</v>
       </c>
@@ -6144,8 +6234,11 @@
       <c r="E236" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F236" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>235</v>
       </c>
@@ -6158,8 +6251,11 @@
       <c r="E237" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F237" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>236</v>
       </c>
@@ -6172,8 +6268,11 @@
       <c r="E238" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F238" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>237</v>
       </c>
@@ -6186,8 +6285,11 @@
       <c r="E239" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F239" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>238</v>
       </c>
@@ -6198,6 +6300,9 @@
         <v>282</v>
       </c>
       <c r="E240" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F240" s="1" t="s">
         <v>282</v>
       </c>
     </row>

</xml_diff>